<commit_message>
Data analysis for problem 1~3
</commit_message>
<xml_diff>
--- a/第2次 第六章/T3/1-data-image.xlsx
+++ b/第2次 第六章/T3/1-data-image.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\文档\大三上\数值代数\第2次 第六章\T3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A644592-997C-4473-9C5C-7450BC07A025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A64B6F-3B51-4123-9E32-16D523485978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,10 +40,6 @@
     <t>Omega: 1.82</t>
   </si>
   <si>
-    <t>J.AError</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>J.Residual</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -61,6 +57,10 @@
   </si>
   <si>
     <t>SOR.Residual</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>J.Aerror</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -800,7 +800,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>J.AError</c:v>
+                  <c:v>J.Aerror</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2690,8 +2690,29 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Three Methods</a:t>
+              <a:t>J</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>方法、</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>GS</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>方法与</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>SOR</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>方法的误差曲线与残差曲线</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2714,15 +2735,7 @@
           <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'1-data'!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>J.AError</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>J方法 误差</c:v>
           </c:tx>
           <c:spPr>
             <a:ln>
@@ -2880,15 +2893,7 @@
           <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'1-data'!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>J.Residual</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>J方法 残量</c:v>
           </c:tx>
           <c:spPr>
             <a:ln>
@@ -3048,15 +3053,7 @@
           <c:idx val="4"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'1-data'!$B$23</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>GS.AError</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>GS方法 误差</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3208,15 +3205,7 @@
           <c:idx val="5"/>
           <c:order val="3"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'1-data'!$C$23</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>GS.Residual</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>GS方法 残量</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3378,15 +3367,7 @@
           <c:idx val="0"/>
           <c:order val="4"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'1-data'!$B$43</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SOR.Aerror</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>SOR方法 误差</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3573,15 +3554,7 @@
           <c:idx val="1"/>
           <c:order val="5"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'1-data'!$C$43</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SOR.Residual</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>SOR方法 残量</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3934,6 +3907,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -5610,15 +5584,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>101600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>155575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>60325</xdr:rowOff>
+      <xdr:rowOff>53975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5717,16 +5691,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5754,6 +5728,57 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.7959</cdr:x>
+      <cdr:y>0.16898</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.93652</cdr:x>
+      <cdr:y>0.50231</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="文本框 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66369CA6-3A1C-354B-7E71-9DB10EF7167D}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5175250" y="463550"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1200"/>
+            <a:t>矩阵参数 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+            <a:t>n=30</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6055,8 +6080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6076,10 +6101,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -6290,10 +6315,10 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
         <v>8</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -6507,10 +6532,10 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
         <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>